<commit_message>
Deployed a new Form version 3 psa_decomp_bag_pre_wt
I changed the xlsx version 3 from editing to deployed in Kobo, and put new csvs of the latested version.
</commit_message>
<xml_diff>
--- a/column_name_dictionary.xlsx
+++ b/column_name_dictionary.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="names" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" calcOnSave="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>type</t>
   </si>
@@ -77,40 +77,55 @@
     <t>begin_group</t>
   </si>
   <si>
-    <t>dry_wt_group_000</t>
-  </si>
-  <si>
     <t>barcode</t>
   </si>
   <si>
-    <t>decomp_bag_000</t>
-  </si>
-  <si>
     <t>decimal</t>
   </si>
   <si>
-    <t>dry_wt_000</t>
-  </si>
-  <si>
     <t>Total Fresh Wt (grams)</t>
   </si>
   <si>
-    <t>end_group</t>
-  </si>
-  <si>
-    <t>dry_wt_group_001</t>
-  </si>
-  <si>
-    <t>decomp_bag_001</t>
-  </si>
-  <si>
-    <t>dry_wt_001</t>
-  </si>
-  <si>
-    <t>indicates next barcode plus data group is coming</t>
-  </si>
-  <si>
     <t>indicates a barcode and data is coming</t>
+  </si>
+  <si>
+    <t>barcode_bag_000</t>
+  </si>
+  <si>
+    <t>group_000</t>
+  </si>
+  <si>
+    <t>Yield:</t>
+  </si>
+  <si>
+    <t>barcode_yield_000</t>
+  </si>
+  <si>
+    <t>yield_wt_000</t>
+  </si>
+  <si>
+    <t>Groups:</t>
+  </si>
+  <si>
+    <t>Site/farm/code</t>
+  </si>
+  <si>
+    <t>Barcodes coming in always start with 'barcode_'</t>
+  </si>
+  <si>
+    <t>Barcode for decomp bag</t>
+  </si>
+  <si>
+    <t>Decomp Bag Pre Wt</t>
+  </si>
+  <si>
+    <t>fresh_bag_wt_grams_000</t>
+  </si>
+  <si>
+    <t>dry_bag_wt_grams_000</t>
+  </si>
+  <si>
+    <t>pre_bag_wt_grams_000</t>
   </si>
 </sst>
 </file>
@@ -436,76 +451,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.6328125" customWidth="1"/>
+    <col min="1" max="1" width="41.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6328125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -521,74 +537,86 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" t="s">
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B12" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="B17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" t="s">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B18" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Kobo forms for decomp_collect, and psa_field updated with latest csvs
</commit_message>
<xml_diff>
--- a/column_name_dictionary.xlsx
+++ b/column_name_dictionary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
   <si>
     <t>type</t>
   </si>
@@ -126,6 +126,18 @@
   </si>
   <si>
     <t>pre_bag_wt_grams_000</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>decomp_bag_collect_date</t>
+  </si>
+  <si>
+    <t>Date the bags in the form were collected</t>
+  </si>
+  <si>
+    <t>ex; barcode_bag and barcode_yield</t>
   </si>
 </sst>
 </file>
@@ -454,7 +466,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -581,13 +593,30 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="B12" s="2" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>28</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated Form psa_gps for 2021
updated to include 2 reps, added new media image with treatment example, removed subplots, added farm code, comments field at end.
</commit_message>
<xml_diff>
--- a/column_name_dictionary.xlsx
+++ b/column_name_dictionary.xlsx
@@ -15,6 +15,7 @@
     <sheet name="names" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
   <si>
     <t>type</t>
   </si>
@@ -47,24 +48,15 @@
     <t>form_name</t>
   </si>
   <si>
-    <t>Form Name</t>
-  </si>
-  <si>
     <t>form_version</t>
   </si>
   <si>
-    <t>Version</t>
-  </si>
-  <si>
     <t>text</t>
   </si>
   <si>
     <t>code</t>
   </si>
   <si>
-    <t>What is the 3 letter site Code?</t>
-  </si>
-  <si>
     <t>geopoint</t>
   </si>
   <si>
@@ -138,14 +130,61 @@
   </si>
   <si>
     <t>ex; barcode_bag and barcode_yield</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>appearance</t>
+  </si>
+  <si>
+    <t>What is the 3 letter site code?</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>hint</t>
+  </si>
+  <si>
+    <t>relevant</t>
+  </si>
+  <si>
+    <t>media::video</t>
+  </si>
+  <si>
+    <t>media::image</t>
+  </si>
+  <si>
+    <t>calculation</t>
+  </si>
+  <si>
+    <t>psa_farm_history_survey</t>
+  </si>
+  <si>
+    <t>v1.1</t>
+  </si>
+  <si>
+    <t>Form Name Here</t>
+  </si>
+  <si>
+    <t>Version #.# here</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -162,7 +201,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -179,10 +218,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,189 +504,224 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="41.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.6328125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="11.54296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.08984375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" style="1"/>
+    <col min="5" max="5" width="13.81640625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="D1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" s="3"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+      <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="1" t="s">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="1" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="B13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B18" s="2" t="s">
-        <v>25</v>
+      <c r="B18" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>